<commit_message>
Irminger FLM recovered ingest CSV files
Created Irminger recovered ingest CSV files
</commit_message>
<xml_diff>
--- a/GI03FLMB/Omaha_Cal_Info_GI03FLMB_00001.xlsx
+++ b/GI03FLMB/Omaha_Cal_Info_GI03FLMB_00001.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\Ingest sheets\ingestion-csvs\GI03FLMB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1660" windowWidth="24820" windowHeight="13320"/>
+    <workbookView xWindow="1920" yWindow="1665" windowWidth="24825" windowHeight="13320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
     <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -250,12 +255,6 @@
     <t>039° 13.81' W</t>
   </si>
   <si>
-    <t>GI03FLMB-RIM01-01-SIOENG000</t>
-  </si>
-  <si>
-    <t>GI03FLMB-RIS01-01-SIOENG000</t>
-  </si>
-  <si>
     <t>AQD 11973</t>
   </si>
   <si>
@@ -327,6 +326,12 @@
   <si>
     <t>37-12223</t>
   </si>
+  <si>
+    <t>GI03FLMB-FMM01-01-SIOENG000</t>
+  </si>
+  <si>
+    <t>GI03FLMB-FMS01-01-SIOENG000</t>
+  </si>
 </sst>
 </file>
 
@@ -394,6 +399,7 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -415,6 +421,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -790,6 +797,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1083,23 +1093,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="1"/>
-    <col min="3" max="3" width="8.83203125" style="2"/>
-    <col min="4" max="4" width="8.83203125" style="3"/>
-    <col min="5" max="5" width="8.83203125" style="4"/>
-    <col min="6" max="6" width="8.83203125" style="3"/>
-    <col min="7" max="7" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="1025" width="8.83203125" style="1"/>
+    <col min="1" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="8.85546875" style="2"/>
+    <col min="4" max="4" width="8.85546875" style="3"/>
+    <col min="5" max="5" width="8.85546875" style="4"/>
+    <col min="6" max="6" width="8.85546875" style="3"/>
+    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="11" customFormat="1" ht="42">
+    <row r="1" spans="1:13" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="16" customFormat="1">
+    <row r="2" spans="1:13" s="16" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>11</v>
       </c>
@@ -1184,22 +1194,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK100"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21:D22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" style="17" customWidth="1"/>
-    <col min="5" max="6" width="28.33203125" style="17" customWidth="1"/>
-    <col min="7" max="1025" width="8.83203125" style="17"/>
+    <col min="1" max="1" width="31.5703125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" style="17" customWidth="1"/>
+    <col min="5" max="6" width="28.28515625" style="17" customWidth="1"/>
+    <col min="7" max="1025" width="8.85546875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="26" customFormat="1" ht="28">
+    <row r="1" spans="1:1024" s="26" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1024">
+    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>55</v>
       </c>
@@ -2262,7 +2272,7 @@
       <c r="AMI2"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024">
+    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>55</v>
       </c>
@@ -3302,7 +3312,7 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024">
+    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>55</v>
       </c>
@@ -4340,7 +4350,7 @@
       <c r="AMI4"/>
       <c r="AMJ4"/>
     </row>
-    <row r="5" spans="1:1024">
+    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>55</v>
       </c>
@@ -5378,7 +5388,7 @@
       <c r="AMI5"/>
       <c r="AMJ5"/>
     </row>
-    <row r="6" spans="1:1024">
+    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>55</v>
       </c>
@@ -6416,7 +6426,7 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024">
+    <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>55</v>
       </c>
@@ -7454,7 +7464,7 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024">
+    <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>55</v>
       </c>
@@ -8494,7 +8504,7 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024">
+    <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>55</v>
       </c>
@@ -9534,7 +9544,7 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024">
+    <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>55</v>
       </c>
@@ -10574,7 +10584,7 @@
       <c r="AMI10"/>
       <c r="AMJ10"/>
     </row>
-    <row r="11" spans="1:1024">
+    <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>55</v>
       </c>
@@ -11614,7 +11624,7 @@
       <c r="AMI11"/>
       <c r="AMJ11"/>
     </row>
-    <row r="12" spans="1:1024">
+    <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>73</v>
       </c>
@@ -12654,7 +12664,7 @@
       <c r="AMI12"/>
       <c r="AMJ12"/>
     </row>
-    <row r="13" spans="1:1024">
+    <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>73</v>
       </c>
@@ -13692,7 +13702,7 @@
       <c r="AMI13"/>
       <c r="AMJ13"/>
     </row>
-    <row r="14" spans="1:1024">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>73</v>
       </c>
@@ -14730,7 +14740,7 @@
       <c r="AMI14"/>
       <c r="AMJ14"/>
     </row>
-    <row r="15" spans="1:1024">
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>73</v>
       </c>
@@ -15768,7 +15778,7 @@
       <c r="AMI15"/>
       <c r="AMJ15"/>
     </row>
-    <row r="16" spans="1:1024">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>73</v>
       </c>
@@ -16806,7 +16816,7 @@
       <c r="AMI16"/>
       <c r="AMJ16"/>
     </row>
-    <row r="17" spans="1:1024">
+    <row r="17" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>73</v>
       </c>
@@ -17844,7 +17854,7 @@
       <c r="AMI17"/>
       <c r="AMJ17"/>
     </row>
-    <row r="18" spans="1:1024">
+    <row r="18" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>73</v>
       </c>
@@ -18884,7 +18894,7 @@
       <c r="AMI18"/>
       <c r="AMJ18"/>
     </row>
-    <row r="19" spans="1:1024">
+    <row r="19" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>39</v>
       </c>
@@ -19924,7 +19934,7 @@
       <c r="AMI19"/>
       <c r="AMJ19"/>
     </row>
-    <row r="20" spans="1:1024">
+    <row r="20" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>39</v>
       </c>
@@ -20964,7 +20974,7 @@
       <c r="AMI20"/>
       <c r="AMJ20"/>
     </row>
-    <row r="21" spans="1:1024">
+    <row r="21" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>39</v>
       </c>
@@ -22002,7 +22012,7 @@
       <c r="AMI21"/>
       <c r="AMJ21"/>
     </row>
-    <row r="22" spans="1:1024">
+    <row r="22" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>56</v>
       </c>
@@ -23042,7 +23052,7 @@
       <c r="AMI22"/>
       <c r="AMJ22"/>
     </row>
-    <row r="23" spans="1:1024">
+    <row r="23" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>56</v>
       </c>
@@ -24080,7 +24090,7 @@
       <c r="AMI23"/>
       <c r="AMJ23"/>
     </row>
-    <row r="24" spans="1:1024">
+    <row r="24" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>56</v>
       </c>
@@ -25118,7 +25128,7 @@
       <c r="AMI24"/>
       <c r="AMJ24"/>
     </row>
-    <row r="25" spans="1:1024">
+    <row r="25" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>56</v>
       </c>
@@ -26156,7 +26166,7 @@
       <c r="AMI25"/>
       <c r="AMJ25"/>
     </row>
-    <row r="26" spans="1:1024">
+    <row r="26" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>56</v>
       </c>
@@ -27194,7 +27204,7 @@
       <c r="AMI26"/>
       <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1024">
+    <row r="27" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>56</v>
       </c>
@@ -28232,7 +28242,7 @@
       <c r="AMI27"/>
       <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024">
+    <row r="28" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>56</v>
       </c>
@@ -29270,7 +29280,7 @@
       <c r="AMI28"/>
       <c r="AMJ28"/>
     </row>
-    <row r="29" spans="1:1024">
+    <row r="29" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>56</v>
       </c>
@@ -30308,7 +30318,7 @@
       <c r="AMI29"/>
       <c r="AMJ29"/>
     </row>
-    <row r="30" spans="1:1024">
+    <row r="30" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>56</v>
       </c>
@@ -31346,7 +31356,7 @@
       <c r="AMI30"/>
       <c r="AMJ30"/>
     </row>
-    <row r="31" spans="1:1024">
+    <row r="31" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>57</v>
       </c>
@@ -31357,7 +31367,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>52</v>
@@ -32386,7 +32396,7 @@
       <c r="AMI31"/>
       <c r="AMJ31"/>
     </row>
-    <row r="32" spans="1:1024">
+    <row r="32" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>57</v>
       </c>
@@ -32397,7 +32407,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>40</v>
@@ -33424,7 +33434,7 @@
       <c r="AMI32"/>
       <c r="AMJ32"/>
     </row>
-    <row r="33" spans="1:1024">
+    <row r="33" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>57</v>
       </c>
@@ -33435,7 +33445,7 @@
         <v>1</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>41</v>
@@ -34462,7 +34472,7 @@
       <c r="AMI33"/>
       <c r="AMJ33"/>
     </row>
-    <row r="34" spans="1:1024">
+    <row r="34" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>57</v>
       </c>
@@ -34473,7 +34483,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>53</v>
@@ -35500,7 +35510,7 @@
       <c r="AMI34"/>
       <c r="AMJ34"/>
     </row>
-    <row r="35" spans="1:1024">
+    <row r="35" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>58</v>
       </c>
@@ -35511,7 +35521,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>52</v>
@@ -36540,7 +36550,7 @@
       <c r="AMI35"/>
       <c r="AMJ35"/>
     </row>
-    <row r="36" spans="1:1024">
+    <row r="36" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>58</v>
       </c>
@@ -36551,7 +36561,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>40</v>
@@ -37578,7 +37588,7 @@
       <c r="AMI36"/>
       <c r="AMJ36"/>
     </row>
-    <row r="37" spans="1:1024">
+    <row r="37" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>58</v>
       </c>
@@ -37589,7 +37599,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>41</v>
@@ -38616,7 +38626,7 @@
       <c r="AMI37"/>
       <c r="AMJ37"/>
     </row>
-    <row r="38" spans="1:1024">
+    <row r="38" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>58</v>
       </c>
@@ -38627,7 +38637,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>53</v>
@@ -39654,7 +39664,7 @@
       <c r="AMI38"/>
       <c r="AMJ38"/>
     </row>
-    <row r="39" spans="1:1024">
+    <row r="39" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>59</v>
       </c>
@@ -39665,7 +39675,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>52</v>
@@ -40694,7 +40704,7 @@
       <c r="AMI39"/>
       <c r="AMJ39"/>
     </row>
-    <row r="40" spans="1:1024">
+    <row r="40" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>59</v>
       </c>
@@ -40705,7 +40715,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>40</v>
@@ -41732,7 +41742,7 @@
       <c r="AMI40"/>
       <c r="AMJ40"/>
     </row>
-    <row r="41" spans="1:1024">
+    <row r="41" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>59</v>
       </c>
@@ -41743,7 +41753,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>41</v>
@@ -42770,7 +42780,7 @@
       <c r="AMI41"/>
       <c r="AMJ41"/>
     </row>
-    <row r="42" spans="1:1024">
+    <row r="42" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>59</v>
       </c>
@@ -42781,7 +42791,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>53</v>
@@ -43808,7 +43818,7 @@
       <c r="AMI42"/>
       <c r="AMJ42"/>
     </row>
-    <row r="43" spans="1:1024">
+    <row r="43" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>60</v>
       </c>
@@ -43819,7 +43829,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E43" s="18" t="s">
         <v>52</v>
@@ -44848,7 +44858,7 @@
       <c r="AMI43"/>
       <c r="AMJ43"/>
     </row>
-    <row r="44" spans="1:1024">
+    <row r="44" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>60</v>
       </c>
@@ -44859,7 +44869,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E44" s="18" t="s">
         <v>40</v>
@@ -45886,7 +45896,7 @@
       <c r="AMI44"/>
       <c r="AMJ44"/>
     </row>
-    <row r="45" spans="1:1024">
+    <row r="45" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>60</v>
       </c>
@@ -45897,7 +45907,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E45" s="18" t="s">
         <v>41</v>
@@ -46924,7 +46934,7 @@
       <c r="AMI45"/>
       <c r="AMJ45"/>
     </row>
-    <row r="46" spans="1:1024">
+    <row r="46" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>60</v>
       </c>
@@ -46935,7 +46945,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E46" s="18" t="s">
         <v>53</v>
@@ -47962,7 +47972,7 @@
       <c r="AMI46"/>
       <c r="AMJ46"/>
     </row>
-    <row r="47" spans="1:1024">
+    <row r="47" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>61</v>
       </c>
@@ -47973,7 +47983,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E47" s="18" t="s">
         <v>52</v>
@@ -49002,7 +49012,7 @@
       <c r="AMI47"/>
       <c r="AMJ47"/>
     </row>
-    <row r="48" spans="1:1024">
+    <row r="48" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>61</v>
       </c>
@@ -49013,7 +49023,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E48" s="18" t="s">
         <v>40</v>
@@ -50040,7 +50050,7 @@
       <c r="AMI48"/>
       <c r="AMJ48"/>
     </row>
-    <row r="49" spans="1:1024">
+    <row r="49" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>61</v>
       </c>
@@ -50051,7 +50061,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E49" s="18" t="s">
         <v>41</v>
@@ -51078,7 +51088,7 @@
       <c r="AMI49"/>
       <c r="AMJ49"/>
     </row>
-    <row r="50" spans="1:1024">
+    <row r="50" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>61</v>
       </c>
@@ -51089,7 +51099,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E50" s="18" t="s">
         <v>53</v>
@@ -52116,7 +52126,7 @@
       <c r="AMI50"/>
       <c r="AMJ50"/>
     </row>
-    <row r="51" spans="1:1024">
+    <row r="51" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
         <v>62</v>
       </c>
@@ -52127,7 +52137,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E51" s="18" t="s">
         <v>52</v>
@@ -53156,7 +53166,7 @@
       <c r="AMI51"/>
       <c r="AMJ51"/>
     </row>
-    <row r="52" spans="1:1024">
+    <row r="52" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>62</v>
       </c>
@@ -53167,7 +53177,7 @@
         <v>1</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E52" s="18" t="s">
         <v>40</v>
@@ -54194,7 +54204,7 @@
       <c r="AMI52"/>
       <c r="AMJ52"/>
     </row>
-    <row r="53" spans="1:1024">
+    <row r="53" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
         <v>62</v>
       </c>
@@ -54205,7 +54215,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E53" s="18" t="s">
         <v>41</v>
@@ -55232,7 +55242,7 @@
       <c r="AMI53"/>
       <c r="AMJ53"/>
     </row>
-    <row r="54" spans="1:1024">
+    <row r="54" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>62</v>
       </c>
@@ -55243,7 +55253,7 @@
         <v>1</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E54" s="18" t="s">
         <v>53</v>
@@ -56270,7 +56280,7 @@
       <c r="AMI54"/>
       <c r="AMJ54"/>
     </row>
-    <row r="55" spans="1:1024">
+    <row r="55" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
         <v>63</v>
       </c>
@@ -56281,7 +56291,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E55" s="18" t="s">
         <v>52</v>
@@ -57310,7 +57320,7 @@
       <c r="AMI55"/>
       <c r="AMJ55"/>
     </row>
-    <row r="56" spans="1:1024">
+    <row r="56" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
         <v>63</v>
       </c>
@@ -57321,7 +57331,7 @@
         <v>1</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E56" s="18" t="s">
         <v>40</v>
@@ -58348,7 +58358,7 @@
       <c r="AMI56"/>
       <c r="AMJ56"/>
     </row>
-    <row r="57" spans="1:1024">
+    <row r="57" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
         <v>63</v>
       </c>
@@ -58359,7 +58369,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E57" s="18" t="s">
         <v>41</v>
@@ -59386,7 +59396,7 @@
       <c r="AMI57"/>
       <c r="AMJ57"/>
     </row>
-    <row r="58" spans="1:1024">
+    <row r="58" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>63</v>
       </c>
@@ -59397,7 +59407,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="27" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E58" s="18" t="s">
         <v>53</v>
@@ -60424,7 +60434,7 @@
       <c r="AMI58"/>
       <c r="AMJ58"/>
     </row>
-    <row r="59" spans="1:1024">
+    <row r="59" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
         <v>64</v>
       </c>
@@ -60435,7 +60445,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E59" s="18" t="s">
         <v>52</v>
@@ -61464,7 +61474,7 @@
       <c r="AMI59"/>
       <c r="AMJ59"/>
     </row>
-    <row r="60" spans="1:1024">
+    <row r="60" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>64</v>
       </c>
@@ -61475,7 +61485,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E60" s="18" t="s">
         <v>40</v>
@@ -62502,7 +62512,7 @@
       <c r="AMI60"/>
       <c r="AMJ60"/>
     </row>
-    <row r="61" spans="1:1024">
+    <row r="61" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>64</v>
       </c>
@@ -62513,7 +62523,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E61" s="18" t="s">
         <v>41</v>
@@ -63540,7 +63550,7 @@
       <c r="AMI61"/>
       <c r="AMJ61"/>
     </row>
-    <row r="62" spans="1:1024">
+    <row r="62" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
         <v>64</v>
       </c>
@@ -63551,7 +63561,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>53</v>
@@ -64578,7 +64588,7 @@
       <c r="AMI62"/>
       <c r="AMJ62"/>
     </row>
-    <row r="63" spans="1:1024">
+    <row r="63" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
         <v>65</v>
       </c>
@@ -64589,7 +64599,7 @@
         <v>1</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E63" s="18" t="s">
         <v>52</v>
@@ -65618,7 +65628,7 @@
       <c r="AMI63"/>
       <c r="AMJ63"/>
     </row>
-    <row r="64" spans="1:1024">
+    <row r="64" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>65</v>
       </c>
@@ -65629,7 +65639,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E64" s="18" t="s">
         <v>40</v>
@@ -66656,7 +66666,7 @@
       <c r="AMI64"/>
       <c r="AMJ64"/>
     </row>
-    <row r="65" spans="1:1025">
+    <row r="65" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
         <v>65</v>
       </c>
@@ -66667,7 +66677,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E65" s="18" t="s">
         <v>41</v>
@@ -67694,7 +67704,7 @@
       <c r="AMI65"/>
       <c r="AMJ65"/>
     </row>
-    <row r="66" spans="1:1025">
+    <row r="66" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
         <v>65</v>
       </c>
@@ -67705,7 +67715,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E66" s="18" t="s">
         <v>53</v>
@@ -68732,7 +68742,7 @@
       <c r="AMI66"/>
       <c r="AMJ66"/>
     </row>
-    <row r="67" spans="1:1025" s="21" customFormat="1">
+    <row r="67" spans="1:1025" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
         <v>70</v>
       </c>
@@ -68743,7 +68753,7 @@
         <v>1</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E67" s="21" t="s">
         <v>52</v>
@@ -68755,7 +68765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:1025">
+    <row r="68" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>70</v>
       </c>
@@ -68766,7 +68776,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>40</v>
@@ -69793,7 +69803,7 @@
       <c r="AMI68"/>
       <c r="AMJ68"/>
     </row>
-    <row r="69" spans="1:1025">
+    <row r="69" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
         <v>70</v>
       </c>
@@ -69804,7 +69814,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E69" s="18" t="s">
         <v>41</v>
@@ -70831,7 +70841,7 @@
       <c r="AMI69"/>
       <c r="AMJ69"/>
     </row>
-    <row r="70" spans="1:1025">
+    <row r="70" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
         <v>70</v>
       </c>
@@ -70842,7 +70852,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E70" s="18" t="s">
         <v>53</v>
@@ -71869,7 +71879,7 @@
       <c r="AMI70"/>
       <c r="AMJ70"/>
     </row>
-    <row r="71" spans="1:1025">
+    <row r="71" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
         <v>71</v>
       </c>
@@ -71880,7 +71890,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>52</v>
@@ -72909,7 +72919,7 @@
       <c r="AMI71"/>
       <c r="AMJ71"/>
     </row>
-    <row r="72" spans="1:1025">
+    <row r="72" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>71</v>
       </c>
@@ -72920,7 +72930,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E72" s="18" t="s">
         <v>40</v>
@@ -73947,7 +73957,7 @@
       <c r="AMI72"/>
       <c r="AMJ72"/>
     </row>
-    <row r="73" spans="1:1025">
+    <row r="73" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
         <v>71</v>
       </c>
@@ -73958,7 +73968,7 @@
         <v>1</v>
       </c>
       <c r="D73" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E73" s="18" t="s">
         <v>41</v>
@@ -74985,7 +74995,7 @@
       <c r="AMI73"/>
       <c r="AMJ73"/>
     </row>
-    <row r="74" spans="1:1025">
+    <row r="74" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
         <v>71</v>
       </c>
@@ -74996,7 +75006,7 @@
         <v>1</v>
       </c>
       <c r="D74" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E74" s="18" t="s">
         <v>53</v>
@@ -76023,7 +76033,7 @@
       <c r="AMI74"/>
       <c r="AMJ74"/>
     </row>
-    <row r="75" spans="1:1025">
+    <row r="75" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
         <v>72</v>
       </c>
@@ -76034,7 +76044,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>52</v>
@@ -77063,7 +77073,7 @@
       <c r="AMI75"/>
       <c r="AMJ75"/>
     </row>
-    <row r="76" spans="1:1025">
+    <row r="76" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
         <v>72</v>
       </c>
@@ -77074,7 +77084,7 @@
         <v>1</v>
       </c>
       <c r="D76" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E76" s="18" t="s">
         <v>40</v>
@@ -78101,7 +78111,7 @@
       <c r="AMI76"/>
       <c r="AMJ76"/>
     </row>
-    <row r="77" spans="1:1025">
+    <row r="77" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>72</v>
       </c>
@@ -78112,7 +78122,7 @@
         <v>1</v>
       </c>
       <c r="D77" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E77" s="18" t="s">
         <v>41</v>
@@ -79139,7 +79149,7 @@
       <c r="AMI77"/>
       <c r="AMJ77"/>
     </row>
-    <row r="78" spans="1:1025">
+    <row r="78" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
         <v>72</v>
       </c>
@@ -79150,7 +79160,7 @@
         <v>1</v>
       </c>
       <c r="D78" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E78" s="18" t="s">
         <v>53</v>
@@ -80177,9 +80187,9 @@
       <c r="AMI78"/>
       <c r="AMJ78"/>
     </row>
-    <row r="79" spans="1:1025" s="30" customFormat="1">
+    <row r="79" spans="1:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B79" s="27" t="s">
         <v>12</v>
@@ -80188,7 +80198,7 @@
         <v>1</v>
       </c>
       <c r="D79" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E79" s="27" t="s">
         <v>52</v>
@@ -80198,9 +80208,9 @@
       </c>
       <c r="AMK79" s="28"/>
     </row>
-    <row r="80" spans="1:1025" s="30" customFormat="1">
+    <row r="80" spans="1:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B80" s="27" t="s">
         <v>12</v>
@@ -80209,7 +80219,7 @@
         <v>1</v>
       </c>
       <c r="D80" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E80" s="27" t="s">
         <v>40</v>
@@ -80219,9 +80229,9 @@
       </c>
       <c r="AMK80" s="28"/>
     </row>
-    <row r="81" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="81" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B81" s="27" t="s">
         <v>12</v>
@@ -80230,7 +80240,7 @@
         <v>1</v>
       </c>
       <c r="D81" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E81" s="27" t="s">
         <v>41</v>
@@ -80240,9 +80250,9 @@
       </c>
       <c r="AMK81" s="28"/>
     </row>
-    <row r="82" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="82" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B82" s="27" t="s">
         <v>12</v>
@@ -80251,7 +80261,7 @@
         <v>1</v>
       </c>
       <c r="D82" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E82" s="27" t="s">
         <v>52</v>
@@ -80261,9 +80271,9 @@
       </c>
       <c r="AMK82" s="28"/>
     </row>
-    <row r="83" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="83" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B83" s="27" t="s">
         <v>12</v>
@@ -80272,7 +80282,7 @@
         <v>1</v>
       </c>
       <c r="D83" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E83" s="27" t="s">
         <v>40</v>
@@ -80282,9 +80292,9 @@
       </c>
       <c r="AMK83" s="28"/>
     </row>
-    <row r="84" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="84" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>12</v>
@@ -80293,7 +80303,7 @@
         <v>1</v>
       </c>
       <c r="D84" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E84" s="27" t="s">
         <v>41</v>
@@ -80303,9 +80313,9 @@
       </c>
       <c r="AMK84" s="28"/>
     </row>
-    <row r="85" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="85" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B85" s="27" t="s">
         <v>12</v>
@@ -80314,7 +80324,7 @@
         <v>1</v>
       </c>
       <c r="D85" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E85" s="27" t="s">
         <v>52</v>
@@ -80324,9 +80334,9 @@
       </c>
       <c r="AMK85" s="28"/>
     </row>
-    <row r="86" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="86" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B86" s="27" t="s">
         <v>12</v>
@@ -80335,7 +80345,7 @@
         <v>1</v>
       </c>
       <c r="D86" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E86" s="27" t="s">
         <v>40</v>
@@ -80345,9 +80355,9 @@
       </c>
       <c r="AMK86" s="28"/>
     </row>
-    <row r="87" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="87" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="27" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B87" s="27" t="s">
         <v>12</v>
@@ -80356,7 +80366,7 @@
         <v>1</v>
       </c>
       <c r="D87" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E87" s="27" t="s">
         <v>41</v>
@@ -80366,9 +80376,9 @@
       </c>
       <c r="AMK87" s="28"/>
     </row>
-    <row r="88" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="88" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B88" s="27" t="s">
         <v>12</v>
@@ -80377,7 +80387,7 @@
         <v>1</v>
       </c>
       <c r="D88" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E88" s="27" t="s">
         <v>52</v>
@@ -80387,9 +80397,9 @@
       </c>
       <c r="AMK88" s="28"/>
     </row>
-    <row r="89" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="89" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B89" s="27" t="s">
         <v>12</v>
@@ -80398,7 +80408,7 @@
         <v>1</v>
       </c>
       <c r="D89" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E89" s="27" t="s">
         <v>40</v>
@@ -80408,9 +80418,9 @@
       </c>
       <c r="AMK89" s="28"/>
     </row>
-    <row r="90" spans="1:7 1025:1025" s="30" customFormat="1">
+    <row r="90" spans="1:7 1025:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B90" s="27" t="s">
         <v>12</v>
@@ -80419,7 +80429,7 @@
         <v>1</v>
       </c>
       <c r="D90" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E90" s="27" t="s">
         <v>41</v>
@@ -80429,7 +80439,7 @@
       </c>
       <c r="AMK90" s="28"/>
     </row>
-    <row r="91" spans="1:7 1025:1025">
+    <row r="91" spans="1:7 1025:1025" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
         <v>66</v>
       </c>
@@ -80440,7 +80450,7 @@
         <v>1</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E91" s="17" t="s">
         <v>40</v>
@@ -80452,7 +80462,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:7 1025:1025">
+    <row r="92" spans="1:7 1025:1025" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
         <v>66</v>
       </c>
@@ -80463,7 +80473,7 @@
         <v>1</v>
       </c>
       <c r="D92" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E92" s="17" t="s">
         <v>41</v>
@@ -80473,7 +80483,7 @@
       </c>
       <c r="G92"/>
     </row>
-    <row r="93" spans="1:7 1025:1025">
+    <row r="93" spans="1:7 1025:1025" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>67</v>
       </c>
@@ -80484,7 +80494,7 @@
         <v>1</v>
       </c>
       <c r="D93" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E93" s="17" t="s">
         <v>40</v>
@@ -80496,7 +80506,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:7 1025:1025">
+    <row r="94" spans="1:7 1025:1025" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>67</v>
       </c>
@@ -80507,7 +80517,7 @@
         <v>1</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E94" s="17" t="s">
         <v>41</v>
@@ -80517,7 +80527,7 @@
       </c>
       <c r="G94"/>
     </row>
-    <row r="95" spans="1:7 1025:1025">
+    <row r="95" spans="1:7 1025:1025" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>68</v>
       </c>
@@ -80528,7 +80538,7 @@
         <v>1</v>
       </c>
       <c r="D95" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E95" s="17" t="s">
         <v>40</v>
@@ -80540,7 +80550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:7 1025:1025">
+    <row r="96" spans="1:7 1025:1025" x14ac:dyDescent="0.25">
       <c r="A96" s="17" t="s">
         <v>68</v>
       </c>
@@ -80551,7 +80561,7 @@
         <v>1</v>
       </c>
       <c r="D96" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E96" s="17" t="s">
         <v>41</v>
@@ -80561,7 +80571,7 @@
       </c>
       <c r="G96"/>
     </row>
-    <row r="97" spans="1:1025">
+    <row r="97" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
         <v>69</v>
       </c>
@@ -80572,7 +80582,7 @@
         <v>1</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E97" s="17" t="s">
         <v>40</v>
@@ -80584,7 +80594,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:1025">
+    <row r="98" spans="1:1025" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
         <v>69</v>
       </c>
@@ -80595,7 +80605,7 @@
         <v>1</v>
       </c>
       <c r="D98" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E98" s="17" t="s">
         <v>41</v>
@@ -80605,9 +80615,9 @@
       </c>
       <c r="G98"/>
     </row>
-    <row r="99" spans="1:1025">
-      <c r="A99" s="27" t="s">
-        <v>76</v>
+    <row r="99" spans="1:1025" x14ac:dyDescent="0.25">
+      <c r="A99" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="B99" s="18" t="s">
         <v>12</v>
@@ -80624,9 +80634,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="100" spans="1:1025" s="30" customFormat="1">
-      <c r="A100" s="28" t="s">
-        <v>77</v>
+    <row r="100" spans="1:1025" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="B100" s="27" t="s">
         <v>12</v>

</xml_diff>